<commit_message>
RR -> Piano di Progetto -> Tutte le tabelle di distribuzione ore e ruoli completate. In attesa di verifca
</commit_message>
<xml_diff>
--- a/RR/Esterni/Piano di Progetto/RISORSE_2_PA.xlsx
+++ b/RR/Esterni/Piano di Progetto/RISORSE_2_PA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
   <si>
     <t>Task Code</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Maggiolo Giorgio</t>
   </si>
   <si>
-    <t>Cornaglia Alessandro</t>
-  </si>
-  <si>
     <t>Dalla Pietà Massimo</t>
   </si>
   <si>
@@ -153,27 +150,6 @@
     <t>Ore III Periodo</t>
   </si>
   <si>
-    <t>Totale cad</t>
-  </si>
-  <si>
-    <t>12h</t>
-  </si>
-  <si>
-    <t>VE 8h</t>
-  </si>
-  <si>
-    <t>PR 8h (PA 3.1)</t>
-  </si>
-  <si>
-    <t>PR 6h (PA 4.1) / RE 2h (PA 4.2)</t>
-  </si>
-  <si>
-    <t>PR 8h (PA 3.2)</t>
-  </si>
-  <si>
-    <t>PR 9h (PA 3.2)</t>
-  </si>
-  <si>
     <t>I Periodo</t>
   </si>
   <si>
@@ -183,51 +159,9 @@
     <t>III Periodo</t>
   </si>
   <si>
-    <t>5h circa</t>
-  </si>
-  <si>
-    <t>8h circa</t>
-  </si>
-  <si>
-    <t>RE 4h (PA 5.1)</t>
-  </si>
-  <si>
-    <t>AM 6h (PA 5.1)</t>
-  </si>
-  <si>
-    <t>RE 4h (PA 3.3)</t>
-  </si>
-  <si>
-    <t>VE 5h (PA 3.3)</t>
-  </si>
-  <si>
-    <t>PR 5h (PA 3.2)</t>
-  </si>
-  <si>
     <t>Membro</t>
   </si>
   <si>
-    <t>Ruolo, ore di lavoro per quel ruolo e compito</t>
-  </si>
-  <si>
-    <t>AN 12h (PA1.1)</t>
-  </si>
-  <si>
-    <t>RE 5h (PA 1.2 e 2.0) /PR 7h (PA3.1)</t>
-  </si>
-  <si>
-    <t>VE 10h (PA 1.2) / PR 2h (PA 3.1)</t>
-  </si>
-  <si>
-    <t>AN 6h (PA 1.1) /PR 6h (PA3.1)</t>
-  </si>
-  <si>
-    <t>AM 5h (PA 2.0) / PR 7h (PA3.1)</t>
-  </si>
-  <si>
-    <t>PR 12h (PA 3.1)</t>
-  </si>
-  <si>
     <t>Costo</t>
   </si>
   <si>
@@ -235,9 +169,6 @@
   </si>
   <si>
     <t>Totale</t>
-  </si>
-  <si>
-    <t>AN 12h (PA 1.1)</t>
   </si>
   <si>
     <t>Ore</t>
@@ -262,16 +193,8 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -295,7 +218,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -832,6 +755,69 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -843,7 +829,6 @@
   </cellStyleXfs>
   <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -858,15 +843,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
@@ -882,47 +863,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -954,182 +899,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1479,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG20" sqref="AG20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1508,26 +1317,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="41" t="s">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="F1" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="43" t="s">
-        <v>41</v>
+      <c r="G1" s="38" t="s">
+        <v>40</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
@@ -1544,35 +1353,35 @@
       <c r="M1" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="O1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="42" t="s">
+      <c r="P1" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="43" t="s">
-        <v>70</v>
+      <c r="Q1" s="38" t="s">
+        <v>48</v>
       </c>
       <c r="R1" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:30">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>30</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="36">
+      <c r="E2" s="7"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="31">
         <f t="shared" ref="G2:G15" si="0">SUM(D2:F2)</f>
         <v>30</v>
       </c>
@@ -1599,14 +1408,14 @@
       <c r="N2">
         <v>1</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="10">
+      <c r="P2" s="9">
         <f>SUM(I2:I109)</f>
         <v>15</v>
       </c>
-      <c r="Q2" s="15">
+      <c r="Q2" s="14">
         <f>P2*R2</f>
         <v>450</v>
       </c>
@@ -1615,21 +1424,21 @@
       </c>
     </row>
     <row r="3" spans="1:30">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>10</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="37">
+      <c r="E3" s="8"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="32">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1656,14 +1465,14 @@
       <c r="N3">
         <v>1</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="6">
         <f>SUM(J2:J110)</f>
         <v>11</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="Q3" s="12">
         <f t="shared" ref="Q3:Q6" si="6">P3*R3</f>
         <v>220</v>
       </c>
@@ -1672,17 +1481,17 @@
       </c>
     </row>
     <row r="4" spans="1:30">
-      <c r="A4" s="14"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="10" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>4</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="38">
+      <c r="E4" s="9"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="33">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1709,14 +1518,14 @@
       <c r="N4">
         <v>2</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="6">
         <f>SUM(K2:K111)</f>
         <v>30</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="Q4" s="12">
         <f t="shared" si="6"/>
         <v>750</v>
       </c>
@@ -1725,21 +1534,21 @@
       </c>
     </row>
     <row r="5" spans="1:30">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>5</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="36">
+      <c r="E5" s="7"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="31">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1766,14 +1575,14 @@
       <c r="N5">
         <v>1</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P5" s="6">
         <f>SUM(L2:L112)</f>
         <v>28</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="12">
         <f t="shared" si="6"/>
         <v>420</v>
       </c>
@@ -1782,17 +1591,17 @@
       </c>
     </row>
     <row r="6" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A6" s="35"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="8" t="s">
+      <c r="A6" s="30"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="36">
+      <c r="E6" s="7"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1819,14 +1628,14 @@
       <c r="N6">
         <v>3</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="P6" s="9">
+      <c r="P6" s="8">
         <f>SUM(M2:M113)</f>
         <v>92</v>
       </c>
-      <c r="Q6" s="19">
+      <c r="Q6" s="16">
         <f t="shared" si="6"/>
         <v>2024</v>
       </c>
@@ -1835,23 +1644,23 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>34</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>8</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="39">
+      <c r="F7" s="5"/>
+      <c r="G7" s="34">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
@@ -1875,36 +1684,36 @@
         <f t="shared" si="5"/>
         <v>42</v>
       </c>
-      <c r="O7" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="P7" s="16">
+      <c r="O7" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="P7" s="37">
         <f>SUM(P2:P6)</f>
         <v>176</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="Q7" s="68">
         <f>SUM(Q2:Q6)</f>
         <v>3864</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="8">
+      <c r="D8" s="3"/>
+      <c r="E8" s="7">
         <v>34</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>10</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="31">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
@@ -1930,21 +1739,21 @@
       </c>
     </row>
     <row r="9" spans="1:30">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="3">
+      <c r="D9" s="2"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="2">
         <v>10</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="32">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1968,45 +1777,41 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O9" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="P9" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="48"/>
-      <c r="U9" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="V9" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="W9" s="51"/>
-      <c r="X9" s="52"/>
-      <c r="Y9" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z9" s="51"/>
-      <c r="AA9" s="52"/>
-      <c r="AB9" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC9" s="51"/>
-      <c r="AD9" s="52"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="62"/>
+      <c r="U9" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="V9" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="W9" s="61"/>
+      <c r="X9" s="62"/>
+      <c r="Y9" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z9" s="61"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC9" s="61"/>
+      <c r="AD9" s="62"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="10" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="5">
+      <c r="D10" s="4"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="4">
         <v>4</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="33">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -2030,61 +1835,55 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O10" s="46"/>
-      <c r="P10" s="23" t="s">
+      <c r="O10" s="60"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="19"/>
+      <c r="U10" s="64"/>
+      <c r="V10" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="W10" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="X10" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="Q10" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="R10" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="U10" s="53"/>
-      <c r="V10" s="54" t="s">
+      <c r="Y10" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="W10" s="55" t="s">
-        <v>74</v>
-      </c>
-      <c r="X10" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y10" s="54" t="s">
+      <c r="Z10" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA10" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB10" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="Z10" s="55" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA10" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB10" s="54" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC10" s="55" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD10" s="56" t="s">
-        <v>75</v>
+      <c r="AC10" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD10" s="67" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:30">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="8">
+      <c r="D11" s="3"/>
+      <c r="E11" s="7">
         <v>6</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="36">
+      <c r="F11" s="3"/>
+      <c r="G11" s="31">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -2108,65 +1907,57 @@
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="O11" s="29" t="s">
+      <c r="O11" s="24"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="25"/>
+      <c r="U11" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="P11" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q11" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="R11" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="U11" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="V11" s="58" t="s">
+      <c r="V11" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="W11" s="59">
+      <c r="W11" s="42">
         <v>12</v>
       </c>
-      <c r="X11" s="60" t="s">
+      <c r="X11" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="Y11" s="58" t="s">
+      <c r="Y11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="Z11" s="59">
+      <c r="Z11" s="42">
         <v>8</v>
       </c>
-      <c r="AA11" s="60" t="s">
+      <c r="AA11" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="AB11" s="58" t="s">
+      <c r="AB11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AC11" s="59">
+      <c r="AC11" s="42">
         <v>5</v>
       </c>
-      <c r="AD11" s="60" t="s">
+      <c r="AD11" s="43" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:30">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="9">
+      <c r="D12" s="2"/>
+      <c r="E12" s="8">
         <v>8</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="37">
+      <c r="F12" s="2"/>
+      <c r="G12" s="32">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -2190,41 +1981,33 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O12" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="P12" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="R12" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="U12" s="61"/>
-      <c r="V12" s="62"/>
-      <c r="W12" s="63"/>
-      <c r="X12" s="64"/>
-      <c r="Y12" s="62"/>
-      <c r="Z12" s="63"/>
-      <c r="AA12" s="64"/>
-      <c r="AB12" s="62"/>
-      <c r="AC12" s="63"/>
-      <c r="AD12" s="73"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="27"/>
+      <c r="U12" s="44"/>
+      <c r="V12" s="45"/>
+      <c r="W12" s="46"/>
+      <c r="X12" s="47"/>
+      <c r="Y12" s="45"/>
+      <c r="Z12" s="46"/>
+      <c r="AA12" s="47"/>
+      <c r="AB12" s="45"/>
+      <c r="AC12" s="46"/>
+      <c r="AD12" s="56"/>
     </row>
     <row r="13" spans="1:30">
-      <c r="A13" s="14"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="10" t="s">
+      <c r="A13" s="13"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="10">
+      <c r="D13" s="4"/>
+      <c r="E13" s="9">
         <v>2</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="38">
+      <c r="F13" s="4"/>
+      <c r="G13" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2248,65 +2031,57 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O13" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q13" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="R13" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="U13" s="57" t="s">
+      <c r="O13" s="26"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="27"/>
+      <c r="U13" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="V13" s="58" t="s">
+      <c r="V13" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="W13" s="59">
+      <c r="W13" s="42">
         <v>5</v>
       </c>
-      <c r="X13" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y13" s="58" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z13" s="59">
+      <c r="X13" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y13" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z13" s="42">
         <v>8</v>
       </c>
-      <c r="AA13" s="60" t="s">
+      <c r="AA13" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="AB13" s="58" t="s">
+      <c r="AB13" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AC13" s="59">
+      <c r="AC13" s="42">
         <v>5</v>
       </c>
-      <c r="AD13" s="60" t="s">
+      <c r="AD13" s="43" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:30">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="4">
+      <c r="D14" s="3"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="3">
         <v>4</v>
       </c>
-      <c r="G14" s="36">
+      <c r="G14" s="31">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -2330,49 +2105,41 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O14" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="P14" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q14" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="R14" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="U14" s="57"/>
-      <c r="V14" s="58" t="s">
+      <c r="O14" s="26"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="27"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="W14" s="59">
+      <c r="W14" s="42">
         <v>7</v>
       </c>
-      <c r="X14" s="60" t="s">
+      <c r="X14" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="Y14" s="58"/>
-      <c r="Z14" s="59"/>
-      <c r="AA14" s="60"/>
-      <c r="AB14" s="58"/>
-      <c r="AC14" s="59"/>
-      <c r="AD14" s="60"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="42"/>
+      <c r="AA14" s="43"/>
+      <c r="AB14" s="41"/>
+      <c r="AC14" s="42"/>
+      <c r="AD14" s="43"/>
     </row>
     <row r="15" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A15" s="35"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="69"/>
+      <c r="B15" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="4">
+      <c r="D15" s="70"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="70">
         <v>6</v>
       </c>
-      <c r="G15" s="36">
+      <c r="G15" s="72">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -2396,319 +2163,286 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O15" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="P15" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q15" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="R15" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="U15" s="65" t="s">
-        <v>76</v>
-      </c>
-      <c r="V15" s="66" t="s">
+      <c r="O15" s="26"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="27"/>
+      <c r="U15" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="V15" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="W15" s="67">
+      <c r="W15" s="50">
         <v>6</v>
       </c>
-      <c r="X15" s="68" t="s">
+      <c r="X15" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="Y15" s="66" t="s">
+      <c r="Y15" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="Z15" s="67">
+      <c r="Z15" s="50">
         <v>8</v>
       </c>
-      <c r="AA15" s="74" t="s">
+      <c r="AA15" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="AB15" s="66" t="s">
+      <c r="AB15" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AC15" s="67">
+      <c r="AC15" s="50">
         <v>5</v>
       </c>
-      <c r="AD15" s="74" t="s">
+      <c r="AD15" s="57" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A16" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16">
+      <c r="O16" s="26"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="27"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="W16" s="46">
+        <v>6</v>
+      </c>
+      <c r="X16" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y16" s="45"/>
+      <c r="Z16" s="46"/>
+      <c r="AA16" s="47"/>
+      <c r="AB16" s="45"/>
+      <c r="AC16" s="46"/>
+      <c r="AD16" s="47"/>
+    </row>
+    <row r="17" spans="1:30" ht="15.75" thickBot="1">
+      <c r="A17" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="75">
         <f>SUM(D2:D15)</f>
         <v>84</v>
       </c>
-      <c r="E16" s="16">
-        <f t="shared" ref="E16:G16" si="7">SUM(E2:E15)</f>
+      <c r="E17" s="75">
+        <f>SUM(E2:E15)</f>
         <v>58</v>
       </c>
-      <c r="F16" s="16">
-        <f t="shared" si="7"/>
+      <c r="F17" s="75">
+        <f>SUM(F2:F15)</f>
         <v>34</v>
       </c>
-      <c r="G16" s="17">
-        <f t="shared" si="7"/>
+      <c r="G17" s="75">
+        <f>SUM(G2:G15)</f>
         <v>176</v>
       </c>
-      <c r="O16" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q16" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="R16" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="U16" s="61"/>
-      <c r="V16" s="62" t="s">
+      <c r="O17" s="28"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="29"/>
+      <c r="U17" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="V17" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="W17" s="42">
+        <v>10</v>
+      </c>
+      <c r="X17" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y17" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="W16" s="63">
-        <v>6</v>
-      </c>
-      <c r="X16" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y16" s="62"/>
-      <c r="Z16" s="63"/>
-      <c r="AA16" s="64"/>
-      <c r="AB16" s="62"/>
-      <c r="AC16" s="63"/>
-      <c r="AD16" s="64"/>
-    </row>
-    <row r="17" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A17" s="1"/>
-      <c r="O17" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="P17" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q17" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="R17" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="U17" s="57" t="s">
-        <v>38</v>
-      </c>
-      <c r="V17" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="W17" s="59">
-        <v>10</v>
-      </c>
-      <c r="X17" s="75" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y17" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z17" s="67">
+      <c r="Z17" s="50">
         <v>8</v>
       </c>
-      <c r="AA17" s="68" t="s">
+      <c r="AA17" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="AB17" s="58" t="s">
+      <c r="AB17" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="AC17" s="59">
+      <c r="AC17" s="42">
         <v>4</v>
       </c>
-      <c r="AD17" s="60" t="s">
+      <c r="AD17" s="43" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="15.75" thickBot="1">
-      <c r="O18" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="P18" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q18" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="R18" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="U18" s="57"/>
-      <c r="V18" s="58" t="s">
+      <c r="O18" s="21"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="23"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="W18" s="59">
+      <c r="W18" s="42">
         <v>2</v>
       </c>
-      <c r="X18" s="60" t="s">
+      <c r="X18" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="Y18" s="58"/>
-      <c r="Z18" s="59"/>
-      <c r="AA18" s="60"/>
-      <c r="AB18" s="58"/>
-      <c r="AC18" s="59"/>
-      <c r="AD18" s="60"/>
+      <c r="Y18" s="41"/>
+      <c r="Z18" s="42"/>
+      <c r="AA18" s="43"/>
+      <c r="AB18" s="41"/>
+      <c r="AC18" s="42"/>
+      <c r="AD18" s="43"/>
     </row>
     <row r="19" spans="1:30">
-      <c r="U19" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="V19" s="66" t="s">
+      <c r="U19" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="V19" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="W19" s="67">
+      <c r="W19" s="50">
         <v>5</v>
       </c>
-      <c r="X19" s="68" t="s">
+      <c r="X19" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="Y19" s="66" t="s">
+      <c r="Y19" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="Z19" s="67">
+      <c r="Z19" s="50">
         <v>9</v>
       </c>
-      <c r="AA19" s="68" t="s">
+      <c r="AA19" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="AB19" s="66" t="s">
+      <c r="AB19" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="AC19" s="67">
+      <c r="AC19" s="50">
         <v>6</v>
       </c>
-      <c r="AD19" s="68" t="s">
+      <c r="AD19" s="51" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:30">
-      <c r="U20" s="61"/>
-      <c r="V20" s="62" t="s">
+      <c r="U20" s="44"/>
+      <c r="V20" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="W20" s="63">
+      <c r="W20" s="46">
         <v>7</v>
       </c>
-      <c r="X20" s="64" t="s">
+      <c r="X20" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="Y20" s="62"/>
-      <c r="Z20" s="63"/>
-      <c r="AA20" s="64"/>
-      <c r="AB20" s="62"/>
-      <c r="AC20" s="63"/>
-      <c r="AD20" s="64"/>
+      <c r="Y20" s="45"/>
+      <c r="Z20" s="46"/>
+      <c r="AA20" s="47"/>
+      <c r="AB20" s="45"/>
+      <c r="AC20" s="46"/>
+      <c r="AD20" s="47"/>
     </row>
     <row r="21" spans="1:30">
-      <c r="U21" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="V21" s="58" t="s">
+      <c r="U21" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="V21" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="W21" s="59">
+      <c r="W21" s="42">
         <v>12</v>
       </c>
-      <c r="X21" s="60" t="s">
+      <c r="X21" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="Y21" s="58" t="s">
+      <c r="Y21" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="Z21" s="59">
+      <c r="Z21" s="42">
         <v>9</v>
       </c>
-      <c r="AA21" s="75" t="s">
+      <c r="AA21" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="AB21" s="58" t="s">
+      <c r="AB21" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="AC21" s="59">
+      <c r="AC21" s="42">
         <v>4</v>
       </c>
-      <c r="AD21" s="75" t="s">
+      <c r="AD21" s="58" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:30">
-      <c r="U22" s="57"/>
-      <c r="V22" s="58"/>
-      <c r="W22" s="59"/>
-      <c r="X22" s="60"/>
-      <c r="Y22" s="58"/>
-      <c r="Z22" s="59"/>
-      <c r="AA22" s="60"/>
-      <c r="AB22" s="58"/>
-      <c r="AC22" s="59"/>
-      <c r="AD22" s="60"/>
+      <c r="U22" s="40"/>
+      <c r="V22" s="41"/>
+      <c r="W22" s="42"/>
+      <c r="X22" s="43"/>
+      <c r="Y22" s="41"/>
+      <c r="Z22" s="42"/>
+      <c r="AA22" s="43"/>
+      <c r="AB22" s="41"/>
+      <c r="AC22" s="42"/>
+      <c r="AD22" s="43"/>
     </row>
     <row r="23" spans="1:30">
-      <c r="O23" s="2"/>
-      <c r="U23" s="65" t="s">
+      <c r="O23" s="1"/>
+      <c r="U23" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="V23" s="66" t="s">
+      <c r="V23" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="W23" s="67">
+      <c r="W23" s="50">
         <v>12</v>
       </c>
-      <c r="X23" s="68" t="s">
+      <c r="X23" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="Y23" s="66" t="s">
+      <c r="Y23" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="Z23" s="67">
+      <c r="Z23" s="50">
         <v>6</v>
       </c>
-      <c r="AA23" s="68" t="s">
+      <c r="AA23" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="AB23" s="66" t="s">
+      <c r="AB23" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AC23" s="67">
+      <c r="AC23" s="50">
         <v>5</v>
       </c>
-      <c r="AD23" s="68" t="s">
+      <c r="AD23" s="51" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:30" ht="15.75" thickBot="1">
-      <c r="U24" s="69"/>
-      <c r="V24" s="70"/>
-      <c r="W24" s="71"/>
-      <c r="X24" s="72"/>
-      <c r="Y24" s="70" t="s">
+      <c r="U24" s="52"/>
+      <c r="V24" s="53"/>
+      <c r="W24" s="54"/>
+      <c r="X24" s="55"/>
+      <c r="Y24" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="Z24" s="71">
+      <c r="Z24" s="54">
         <v>2</v>
       </c>
-      <c r="AA24" s="72" t="s">
+      <c r="AA24" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="AB24" s="70"/>
-      <c r="AC24" s="71"/>
-      <c r="AD24" s="72"/>
+      <c r="AB24" s="53"/>
+      <c r="AC24" s="54"/>
+      <c r="AD24" s="55"/>
     </row>
     <row r="26" spans="1:30">
       <c r="W26">
@@ -2723,7 +2457,7 @@
         <f>SUM(AC11:AC24)</f>
         <v>34</v>
       </c>
-      <c r="AD26" s="2"/>
+      <c r="AD26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2735,27 +2469,27 @@
     <mergeCell ref="Y9:AA9"/>
   </mergeCells>
   <conditionalFormatting sqref="Z26">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="notEqual">
-      <formula>$E$16</formula>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="notEqual">
+      <formula>$E$17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
-      <formula>$E$16</formula>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>$E$17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W26">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="notEqual">
-      <formula>$D$16</formula>
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="notEqual">
+      <formula>$D$17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
-      <formula>$D$16</formula>
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+      <formula>$D$17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC26">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="notEqual">
-      <formula>$F$16</formula>
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="notEqual">
+      <formula>$F$17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
-      <formula>$F$16</formula>
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
+      <formula>$F$17</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modifica al nome del progetto nei file preface.tex. Inoltre modifiche al Piano di Progetto (NON TOCCARE IL CAPITOLO 3)
</commit_message>
<xml_diff>
--- a/RR/Esterni/Piano di Progetto/RISORSE_2_PA.xlsx
+++ b/RR/Esterni/Piano di Progetto/RISORSE_2_PA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
@@ -11,12 +11,12 @@
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="58">
   <si>
     <t>Task Code</t>
   </si>
@@ -184,16 +184,22 @@
   </si>
   <si>
     <t>PA 1.2 e 2.0</t>
+  </si>
+  <si>
+    <t>Carico lavoro</t>
+  </si>
+  <si>
+    <t>Cornaglia Alessandro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,7 +224,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="56">
     <border>
       <left/>
       <right/>
@@ -823,11 +829,111 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -838,7 +944,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
@@ -846,18 +951,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
@@ -899,24 +996,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -934,6 +1013,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -998,6 +1111,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1076,6 +1194,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1110,6 +1229,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1285,14 +1405,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH22" sqref="AH22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="32.140625" customWidth="1"/>
@@ -1314,28 +1434,33 @@
     <col min="24" max="24" width="11.7109375" customWidth="1"/>
     <col min="27" max="27" width="7" customWidth="1"/>
     <col min="30" max="30" width="8.28515625" customWidth="1"/>
+    <col min="32" max="32" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.28515625" customWidth="1"/>
+    <col min="34" max="34" width="11.140625" customWidth="1"/>
+    <col min="35" max="35" width="12.140625" customWidth="1"/>
+    <col min="36" max="36" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="29" t="s">
         <v>40</v>
       </c>
       <c r="I1" t="s">
@@ -1353,21 +1478,21 @@
       <c r="M1" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="O1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="P1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="38" t="s">
+      <c r="Q1" s="29" t="s">
         <v>48</v>
       </c>
       <c r="R1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1381,7 +1506,7 @@
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="31">
+      <c r="G2" s="22">
         <f t="shared" ref="G2:G15" si="0">SUM(D2:F2)</f>
         <v>30</v>
       </c>
@@ -1408,14 +1533,14 @@
       <c r="N2">
         <v>1</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="12" t="s">
         <v>6</v>
       </c>
       <c r="P2" s="9">
         <f>SUM(I2:I109)</f>
         <v>15</v>
       </c>
-      <c r="Q2" s="14">
+      <c r="Q2" s="13">
         <f>P2*R2</f>
         <v>450</v>
       </c>
@@ -1423,8 +1548,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1438,7 +1563,7 @@
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="32">
+      <c r="G3" s="23">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1465,14 +1590,14 @@
       <c r="N3">
         <v>1</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="P3" s="6">
         <f>SUM(J2:J110)</f>
         <v>11</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="Q3" s="11">
         <f t="shared" ref="Q3:Q6" si="6">P3*R3</f>
         <v>220</v>
       </c>
@@ -1480,8 +1605,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
-      <c r="A4" s="13"/>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
       <c r="B4" s="4"/>
       <c r="C4" s="9" t="s">
         <v>6</v>
@@ -1491,7 +1616,7 @@
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="33">
+      <c r="G4" s="24">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1518,14 +1643,14 @@
       <c r="N4">
         <v>2</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="P4" s="6">
         <f>SUM(K2:K111)</f>
         <v>30</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="Q4" s="11">
         <f t="shared" si="6"/>
         <v>750</v>
       </c>
@@ -1533,8 +1658,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1548,7 +1673,7 @@
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="31">
+      <c r="G5" s="22">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1575,14 +1700,14 @@
       <c r="N5">
         <v>1</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="O5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="P5" s="6">
         <f>SUM(L2:L112)</f>
         <v>28</v>
       </c>
-      <c r="Q5" s="12">
+      <c r="Q5" s="11">
         <f t="shared" si="6"/>
         <v>420</v>
       </c>
@@ -1590,8 +1715,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A6" s="30"/>
+    <row r="6" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="21"/>
       <c r="B6" s="3"/>
       <c r="C6" s="7" t="s">
         <v>6</v>
@@ -1601,7 +1726,7 @@
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="31">
+      <c r="G6" s="22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1628,14 +1753,14 @@
       <c r="N6">
         <v>3</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="14" t="s">
         <v>23</v>
       </c>
       <c r="P6" s="8">
         <f>SUM(M2:M113)</f>
         <v>92</v>
       </c>
-      <c r="Q6" s="16">
+      <c r="Q6" s="15">
         <f t="shared" si="6"/>
         <v>2024</v>
       </c>
@@ -1643,8 +1768,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1660,7 +1785,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="34">
+      <c r="G7" s="25">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
@@ -1684,20 +1809,20 @@
         <f t="shared" si="5"/>
         <v>42</v>
       </c>
-      <c r="O7" s="39" t="s">
+      <c r="O7" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="P7" s="37">
+      <c r="P7" s="28">
         <f>SUM(P2:P6)</f>
         <v>176</v>
       </c>
-      <c r="Q7" s="68">
+      <c r="Q7" s="53">
         <f>SUM(Q2:Q6)</f>
         <v>3864</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1713,7 +1838,7 @@
       <c r="F8" s="3">
         <v>10</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="22">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
@@ -1738,8 +1863,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1753,7 +1878,7 @@
       <c r="F9" s="2">
         <v>10</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="23">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1777,31 +1902,36 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O9" s="59"/>
-      <c r="P9" s="61"/>
-      <c r="Q9" s="61"/>
-      <c r="R9" s="62"/>
-      <c r="U9" s="63" t="s">
+      <c r="U9" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="V9" s="59" t="s">
+      <c r="V9" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="W9" s="61"/>
-      <c r="X9" s="62"/>
-      <c r="Y9" s="59" t="s">
+      <c r="W9" s="62"/>
+      <c r="X9" s="63"/>
+      <c r="Y9" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="Z9" s="61"/>
-      <c r="AA9" s="62"/>
-      <c r="AB9" s="59" t="s">
+      <c r="Z9" s="62"/>
+      <c r="AA9" s="63"/>
+      <c r="AB9" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="AC9" s="61"/>
-      <c r="AD9" s="62"/>
+      <c r="AC9" s="62"/>
+      <c r="AD9" s="63"/>
+      <c r="AF9" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG9" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH9" s="62"/>
+      <c r="AI9" s="67"/>
+      <c r="AJ9" s="74"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
       <c r="B10" s="4"/>
       <c r="C10" s="9" t="s">
         <v>6</v>
@@ -1811,7 +1941,7 @@
       <c r="F10" s="4">
         <v>4</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1835,41 +1965,50 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O10" s="60"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="19"/>
-      <c r="U10" s="64"/>
-      <c r="V10" s="65" t="s">
+      <c r="U10" s="66"/>
+      <c r="V10" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="W10" s="66" t="s">
+      <c r="W10" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="X10" s="67" t="s">
+      <c r="X10" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="Y10" s="65" t="s">
+      <c r="Y10" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="Z10" s="66" t="s">
+      <c r="Z10" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="AA10" s="67" t="s">
+      <c r="AA10" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="AB10" s="65" t="s">
+      <c r="AB10" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="AC10" s="66" t="s">
+      <c r="AC10" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="AD10" s="67" t="s">
+      <c r="AD10" s="52" t="s">
         <v>52</v>
       </c>
+      <c r="AF10" s="64"/>
+      <c r="AG10" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH10" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI10" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ10" s="76" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="11" spans="1:30">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1883,7 +2022,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="31">
+      <c r="G11" s="22">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1907,43 +2046,58 @@
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="O11" s="24"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="25"/>
-      <c r="U11" s="40" t="s">
+      <c r="U11" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="V11" s="41" t="s">
+      <c r="V11" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="W11" s="42">
+      <c r="W11" s="33">
         <v>12</v>
       </c>
-      <c r="X11" s="43" t="s">
+      <c r="X11" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Y11" s="41" t="s">
+      <c r="Y11" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="Z11" s="42">
+      <c r="Z11" s="33">
         <v>8</v>
       </c>
-      <c r="AA11" s="43" t="s">
+      <c r="AA11" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="AB11" s="41" t="s">
+      <c r="AB11" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="AC11" s="42">
+      <c r="AC11" s="33">
         <v>5</v>
       </c>
-      <c r="AD11" s="43" t="s">
+      <c r="AD11" s="34" t="s">
         <v>20</v>
       </c>
+      <c r="AF11" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG11" s="9">
+        <f>SUM(W11,W12)</f>
+        <v>12</v>
+      </c>
+      <c r="AH11" s="16">
+        <f>SUM(Z11,Z12)</f>
+        <v>8</v>
+      </c>
+      <c r="AI11" s="68">
+        <f>SUM(AC11,AC12)</f>
+        <v>5</v>
+      </c>
+      <c r="AJ11" s="72">
+        <f>SUM(AG11:AI11)</f>
+        <v>25</v>
+      </c>
     </row>
-    <row r="12" spans="1:30">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1957,7 +2111,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="32">
+      <c r="G12" s="23">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1981,23 +2135,38 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O12" s="26"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="27"/>
-      <c r="U12" s="44"/>
-      <c r="V12" s="45"/>
-      <c r="W12" s="46"/>
-      <c r="X12" s="47"/>
-      <c r="Y12" s="45"/>
-      <c r="Z12" s="46"/>
-      <c r="AA12" s="47"/>
-      <c r="AB12" s="45"/>
-      <c r="AC12" s="46"/>
-      <c r="AD12" s="56"/>
+      <c r="U12" s="35"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="37"/>
+      <c r="X12" s="38"/>
+      <c r="Y12" s="36"/>
+      <c r="Z12" s="37"/>
+      <c r="AA12" s="38"/>
+      <c r="AB12" s="36"/>
+      <c r="AC12" s="37"/>
+      <c r="AD12" s="47"/>
+      <c r="AF12" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG12" s="9">
+        <f>SUM(W13,W14)</f>
+        <v>12</v>
+      </c>
+      <c r="AH12" s="16">
+        <f>SUM(Z14,Z13)</f>
+        <v>8</v>
+      </c>
+      <c r="AI12" s="69">
+        <f>SUM(AC14,AC13)</f>
+        <v>5</v>
+      </c>
+      <c r="AJ12" s="23">
+        <f t="shared" ref="AJ12:AJ17" si="7">SUM(AG12:AI12)</f>
+        <v>25</v>
+      </c>
     </row>
-    <row r="13" spans="1:30">
-      <c r="A13" s="13"/>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
       <c r="B13" s="4"/>
       <c r="C13" s="9" t="s">
         <v>6</v>
@@ -2007,7 +2176,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="33">
+      <c r="G13" s="24">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2031,43 +2200,58 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O13" s="26"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="27"/>
-      <c r="U13" s="40" t="s">
+      <c r="U13" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="V13" s="41" t="s">
+      <c r="V13" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="W13" s="42">
+      <c r="W13" s="33">
         <v>5</v>
       </c>
-      <c r="X13" s="43" t="s">
+      <c r="X13" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="Y13" s="41" t="s">
+      <c r="Y13" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="Z13" s="42">
+      <c r="Z13" s="33">
         <v>8</v>
       </c>
-      <c r="AA13" s="43" t="s">
+      <c r="AA13" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="AB13" s="41" t="s">
+      <c r="AB13" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="AC13" s="42">
+      <c r="AC13" s="33">
         <v>5</v>
       </c>
-      <c r="AD13" s="43" t="s">
+      <c r="AD13" s="34" t="s">
         <v>20</v>
       </c>
+      <c r="AF13" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG13" s="9">
+        <f>SUM(W16,W15)</f>
+        <v>12</v>
+      </c>
+      <c r="AH13" s="16">
+        <f>SUM(Z15,Z16)</f>
+        <v>8</v>
+      </c>
+      <c r="AI13" s="69">
+        <f>SUM(AC15,AC16)</f>
+        <v>5</v>
+      </c>
+      <c r="AJ13" s="25">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
     </row>
-    <row r="14" spans="1:30">
-      <c r="A14" s="30" t="s">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -2081,7 +2265,7 @@
       <c r="F14" s="3">
         <v>4</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G14" s="22">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -2105,41 +2289,56 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O14" s="26"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="27"/>
-      <c r="U14" s="40"/>
-      <c r="V14" s="41" t="s">
+      <c r="U14" s="31"/>
+      <c r="V14" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="W14" s="42">
+      <c r="W14" s="33">
         <v>7</v>
       </c>
-      <c r="X14" s="43" t="s">
+      <c r="X14" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="Y14" s="41"/>
-      <c r="Z14" s="42"/>
-      <c r="AA14" s="43"/>
-      <c r="AB14" s="41"/>
-      <c r="AC14" s="42"/>
-      <c r="AD14" s="43"/>
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="33"/>
+      <c r="AA14" s="34"/>
+      <c r="AB14" s="32"/>
+      <c r="AC14" s="33"/>
+      <c r="AD14" s="34"/>
+      <c r="AF14" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG14" s="9">
+        <f>SUM(W17,W18)</f>
+        <v>12</v>
+      </c>
+      <c r="AH14" s="16">
+        <f>SUM(Z17,Z18)</f>
+        <v>8</v>
+      </c>
+      <c r="AI14" s="69">
+        <f t="shared" ref="AI12:AI17" si="8">SUM(AC14,AC15)</f>
+        <v>5</v>
+      </c>
+      <c r="AJ14" s="25">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
     </row>
-    <row r="15" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A15" s="69"/>
-      <c r="B15" s="70" t="s">
+    <row r="15" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="54"/>
+      <c r="B15" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="71" t="s">
+      <c r="C15" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="70"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="70">
+      <c r="D15" s="55"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="55">
         <v>6</v>
       </c>
-      <c r="G15" s="72">
+      <c r="G15" s="57">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -2163,288 +2362,349 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O15" s="26"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="27"/>
-      <c r="U15" s="48" t="s">
+      <c r="U15" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="V15" s="49" t="s">
+      <c r="V15" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="W15" s="50">
+      <c r="W15" s="41">
         <v>6</v>
       </c>
-      <c r="X15" s="51" t="s">
+      <c r="X15" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="Y15" s="49" t="s">
+      <c r="Y15" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z15" s="50">
+      <c r="Z15" s="41">
         <v>8</v>
       </c>
-      <c r="AA15" s="57" t="s">
+      <c r="AA15" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="AB15" s="49" t="s">
+      <c r="AB15" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="AC15" s="50">
+      <c r="AC15" s="41">
         <v>5</v>
       </c>
-      <c r="AD15" s="57" t="s">
+      <c r="AD15" s="48" t="s">
         <v>21</v>
       </c>
+      <c r="AF15" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG15" s="9">
+        <f>SUM(W19,W20)</f>
+        <v>12</v>
+      </c>
+      <c r="AH15" s="16">
+        <f>SUM(Z19,Z20)</f>
+        <v>9</v>
+      </c>
+      <c r="AI15" s="69">
+        <f>SUM(AC17,AC18)</f>
+        <v>4</v>
+      </c>
+      <c r="AJ15" s="25">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
     </row>
-    <row r="16" spans="1:30" ht="15.75" thickBot="1">
-      <c r="O16" s="26"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="27"/>
-      <c r="U16" s="44"/>
-      <c r="V16" s="45" t="s">
+    <row r="16" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U16" s="35"/>
+      <c r="V16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="W16" s="46">
+      <c r="W16" s="37">
         <v>6</v>
       </c>
-      <c r="X16" s="47" t="s">
+      <c r="X16" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="Y16" s="45"/>
-      <c r="Z16" s="46"/>
-      <c r="AA16" s="47"/>
-      <c r="AB16" s="45"/>
-      <c r="AC16" s="46"/>
-      <c r="AD16" s="47"/>
+      <c r="Y16" s="36"/>
+      <c r="Z16" s="37"/>
+      <c r="AA16" s="38"/>
+      <c r="AB16" s="36"/>
+      <c r="AC16" s="37"/>
+      <c r="AD16" s="38"/>
+      <c r="AF16" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG16" s="9">
+        <f>SUM(W21,W22)</f>
+        <v>12</v>
+      </c>
+      <c r="AH16" s="16">
+        <f>SUM(Z22,Z21)</f>
+        <v>9</v>
+      </c>
+      <c r="AI16" s="69">
+        <f>SUM(AC19,AC20)</f>
+        <v>6</v>
+      </c>
+      <c r="AJ16" s="24">
+        <f t="shared" si="7"/>
+        <v>27</v>
+      </c>
     </row>
-    <row r="17" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A17" s="73" t="s">
+    <row r="17" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="75">
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="60">
         <f>SUM(D2:D15)</f>
         <v>84</v>
       </c>
-      <c r="E17" s="75">
+      <c r="E17" s="60">
         <f>SUM(E2:E15)</f>
         <v>58</v>
       </c>
-      <c r="F17" s="75">
+      <c r="F17" s="60">
         <f>SUM(F2:F15)</f>
         <v>34</v>
       </c>
-      <c r="G17" s="75">
+      <c r="G17" s="60">
         <f>SUM(G2:G15)</f>
         <v>176</v>
       </c>
-      <c r="O17" s="28"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="29"/>
-      <c r="U17" s="40" t="s">
+      <c r="U17" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="V17" s="41" t="s">
+      <c r="V17" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="W17" s="42">
+      <c r="W17" s="33">
         <v>10</v>
       </c>
-      <c r="X17" s="58" t="s">
+      <c r="X17" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="Y17" s="49" t="s">
+      <c r="Y17" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z17" s="50">
+      <c r="Z17" s="41">
         <v>8</v>
       </c>
-      <c r="AA17" s="51" t="s">
+      <c r="AA17" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="AB17" s="41" t="s">
+      <c r="AB17" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="AC17" s="42">
+      <c r="AC17" s="33">
         <v>4</v>
       </c>
-      <c r="AD17" s="43" t="s">
+      <c r="AD17" s="34" t="s">
         <v>21</v>
       </c>
+      <c r="AF17" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG17" s="9">
+        <f>SUM(W23,W24)</f>
+        <v>12</v>
+      </c>
+      <c r="AH17" s="16">
+        <f>SUM(Z24,Z23)</f>
+        <v>8</v>
+      </c>
+      <c r="AI17" s="70">
+        <f>SUM(AC21,AC22)</f>
+        <v>4</v>
+      </c>
+      <c r="AJ17" s="57">
+        <f t="shared" si="7"/>
+        <v>24</v>
+      </c>
     </row>
-    <row r="18" spans="1:30" ht="15.75" thickBot="1">
-      <c r="O18" s="21"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="23"/>
-      <c r="U18" s="40"/>
-      <c r="V18" s="41" t="s">
+    <row r="18" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U18" s="31"/>
+      <c r="V18" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="W18" s="42">
+      <c r="W18" s="33">
         <v>2</v>
       </c>
-      <c r="X18" s="43" t="s">
+      <c r="X18" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="Y18" s="41"/>
-      <c r="Z18" s="42"/>
-      <c r="AA18" s="43"/>
-      <c r="AB18" s="41"/>
-      <c r="AC18" s="42"/>
-      <c r="AD18" s="43"/>
+      <c r="Y18" s="32"/>
+      <c r="Z18" s="33"/>
+      <c r="AA18" s="34"/>
+      <c r="AB18" s="32"/>
+      <c r="AC18" s="33"/>
+      <c r="AD18" s="34"/>
+      <c r="AF18" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG18" s="17">
+        <f t="shared" ref="AG18:AI18" si="9">SUM(AG11:AG17)</f>
+        <v>84</v>
+      </c>
+      <c r="AH18" s="17">
+        <f t="shared" si="9"/>
+        <v>58</v>
+      </c>
+      <c r="AI18" s="71">
+        <f t="shared" si="9"/>
+        <v>34</v>
+      </c>
+      <c r="AJ18" s="73">
+        <f>SUM(AJ11:AJ17)</f>
+        <v>176</v>
+      </c>
     </row>
-    <row r="19" spans="1:30">
-      <c r="U19" s="48" t="s">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="U19" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="V19" s="49" t="s">
+      <c r="V19" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="W19" s="50">
+      <c r="W19" s="41">
         <v>5</v>
       </c>
-      <c r="X19" s="51" t="s">
+      <c r="X19" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="Y19" s="49" t="s">
+      <c r="Y19" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z19" s="50">
+      <c r="Z19" s="41">
         <v>9</v>
       </c>
-      <c r="AA19" s="51" t="s">
+      <c r="AA19" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="AB19" s="49" t="s">
+      <c r="AB19" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="AC19" s="50">
+      <c r="AC19" s="41">
         <v>6</v>
       </c>
-      <c r="AD19" s="51" t="s">
+      <c r="AD19" s="42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
-      <c r="U20" s="44"/>
-      <c r="V20" s="45" t="s">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="U20" s="35"/>
+      <c r="V20" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="W20" s="46">
+      <c r="W20" s="37">
         <v>7</v>
       </c>
-      <c r="X20" s="47" t="s">
+      <c r="X20" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="Y20" s="45"/>
-      <c r="Z20" s="46"/>
-      <c r="AA20" s="47"/>
-      <c r="AB20" s="45"/>
-      <c r="AC20" s="46"/>
-      <c r="AD20" s="47"/>
+      <c r="Y20" s="36"/>
+      <c r="Z20" s="37"/>
+      <c r="AA20" s="38"/>
+      <c r="AB20" s="36"/>
+      <c r="AC20" s="37"/>
+      <c r="AD20" s="38"/>
     </row>
-    <row r="21" spans="1:30">
-      <c r="U21" s="40" t="s">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="U21" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="V21" s="41" t="s">
+      <c r="V21" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="W21" s="42">
+      <c r="W21" s="33">
         <v>12</v>
       </c>
-      <c r="X21" s="43" t="s">
+      <c r="X21" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="Y21" s="41" t="s">
+      <c r="Y21" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="Z21" s="42">
+      <c r="Z21" s="33">
         <v>9</v>
       </c>
-      <c r="AA21" s="58" t="s">
+      <c r="AA21" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="AB21" s="41" t="s">
+      <c r="AB21" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="AC21" s="42">
+      <c r="AC21" s="33">
         <v>4</v>
       </c>
-      <c r="AD21" s="58" t="s">
+      <c r="AD21" s="49" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
-      <c r="U22" s="40"/>
-      <c r="V22" s="41"/>
-      <c r="W22" s="42"/>
-      <c r="X22" s="43"/>
-      <c r="Y22" s="41"/>
-      <c r="Z22" s="42"/>
-      <c r="AA22" s="43"/>
-      <c r="AB22" s="41"/>
-      <c r="AC22" s="42"/>
-      <c r="AD22" s="43"/>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="U22" s="31"/>
+      <c r="V22" s="32"/>
+      <c r="W22" s="33"/>
+      <c r="X22" s="34"/>
+      <c r="Y22" s="32"/>
+      <c r="Z22" s="33"/>
+      <c r="AA22" s="34"/>
+      <c r="AB22" s="32"/>
+      <c r="AC22" s="33"/>
+      <c r="AD22" s="34"/>
+      <c r="AH22" s="1"/>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="O23" s="1"/>
-      <c r="U23" s="48" t="s">
+      <c r="U23" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="V23" s="49" t="s">
+      <c r="V23" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="W23" s="50">
+      <c r="W23" s="41">
         <v>12</v>
       </c>
-      <c r="X23" s="51" t="s">
+      <c r="X23" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="Y23" s="49" t="s">
+      <c r="Y23" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z23" s="50">
+      <c r="Z23" s="41">
         <v>6</v>
       </c>
-      <c r="AA23" s="51" t="s">
+      <c r="AA23" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AB23" s="49" t="s">
+      <c r="AB23" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="AC23" s="50">
+      <c r="AC23" s="41">
         <v>5</v>
       </c>
-      <c r="AD23" s="51" t="s">
+      <c r="AD23" s="42" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="15.75" thickBot="1">
-      <c r="U24" s="52"/>
-      <c r="V24" s="53"/>
-      <c r="W24" s="54"/>
-      <c r="X24" s="55"/>
-      <c r="Y24" s="53" t="s">
+    <row r="24" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U24" s="43"/>
+      <c r="V24" s="44"/>
+      <c r="W24" s="45"/>
+      <c r="X24" s="46"/>
+      <c r="Y24" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="Z24" s="54">
+      <c r="Z24" s="45">
         <v>2</v>
       </c>
-      <c r="AA24" s="55" t="s">
+      <c r="AA24" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="AB24" s="53"/>
-      <c r="AC24" s="54"/>
-      <c r="AD24" s="55"/>
+      <c r="AB24" s="44"/>
+      <c r="AC24" s="45"/>
+      <c r="AD24" s="46"/>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="W26">
         <f>SUM(W11:W23)</f>
         <v>84</v>
@@ -2462,8 +2722,8 @@
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="AB9:AD9"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AI9"/>
     <mergeCell ref="U9:U10"/>
     <mergeCell ref="V9:X9"/>
     <mergeCell ref="Y9:AA9"/>
@@ -2498,24 +2758,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>